<commit_message>
almost completed angular project
</commit_message>
<xml_diff>
--- a/Assignments/Adv/Advertisement_REST_call_details_v3.xlsx
+++ b/Assignments/Adv/Advertisement_REST_call_details_v3.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Xoriant\Training\MainRepo\freshersbatch-jul17\Assignments\Adv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MainRepo\freshersbatch-jul17\Assignments\Adv\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -222,15 +222,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Lucida Console"/>
       <family val="3"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFFF0000"/>
       <name val="Lucida Console"/>
       <family val="3"/>
     </font>
@@ -287,9 +287,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -300,6 +297,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -671,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B2:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,7 +720,7 @@
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -742,7 +742,7 @@
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -762,13 +762,13 @@
       <c r="C5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="4"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -780,7 +780,7 @@
       <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="8" t="s">
         <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -800,7 +800,7 @@
       <c r="C7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>19</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -824,7 +824,7 @@
       <c r="C8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="8" t="s">
         <v>19</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -846,7 +846,7 @@
       <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="8" t="s">
         <v>22</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -866,7 +866,7 @@
       <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -888,7 +888,7 @@
       <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -910,7 +910,7 @@
       <c r="C12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -932,7 +932,7 @@
       <c r="C13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E13" s="2" t="s">
@@ -954,7 +954,7 @@
       <c r="C14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="8" t="s">
         <v>33</v>
       </c>
       <c r="E14" s="2" t="s">
@@ -974,7 +974,7 @@
       <c r="C15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="8" t="s">
         <v>47</v>
       </c>
       <c r="E15" s="2" t="s">
@@ -996,7 +996,7 @@
       <c r="C16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="9" t="s">
         <v>35</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -1016,7 +1016,7 @@
       <c r="C17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -1038,7 +1038,7 @@
       <c r="C18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="8" t="s">
         <v>38</v>
       </c>
       <c r="E18" s="2" t="s">
@@ -1057,41 +1057,41 @@
       <c r="B19" s="3">
         <v>17</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5" t="s">
+      <c r="F19" s="4"/>
+      <c r="G19" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="6">
+      <c r="B20" s="5">
         <v>18</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F20" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="7" t="s">
+      <c r="F20" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="6" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>